<commit_message>
run instances, display gantt, jalon2 cleaning
</commit_message>
<xml_diff>
--- a/outputs/results/results_instance_WPY_realiste_jalon1.xlsx
+++ b/outputs/results/results_instance_WPY_realiste_jalon1.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>21:48</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -511,7 +511,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>14:36</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -539,7 +539,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -567,7 +567,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -595,7 +595,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14:21</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -623,7 +623,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>00:35</t>
+          <t>00:45</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -651,7 +651,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>23:01</t>
+          <t>23:15</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -679,7 +679,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>00:50</t>
+          <t>01:00</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -707,7 +707,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>22:28</t>
+          <t>22:30</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -735,7 +735,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>03:07</t>
+          <t>03:15</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>23:33</t>
+          <t>23:45</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -819,7 +819,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>19:13</t>
+          <t>19:15</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -847,7 +847,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>11:18</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -875,7 +875,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -903,7 +903,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -931,7 +931,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13:43</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -959,7 +959,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -987,7 +987,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>10:31</t>
+          <t>10:45</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>23:01</t>
+          <t>23:15</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>00:49</t>
+          <t>01:00</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12:32</t>
+          <t>12:30</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>03:32</t>
+          <t>03:45</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>03:07</t>
+          <t>03:15</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>21:48</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>23:33</t>
+          <t>23:45</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>21:18</t>
+          <t>21:30</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12:04</t>
+          <t>12:15</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>04:55</t>
+          <t>05:00</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>02:13</t>
+          <t>02:15</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>11:18</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1532,7 +1532,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>DEB_47262_11/08/2022</t>
+          <t>DEB_47262_10/08/2022</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1542,12 +1542,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11/08/2022</t>
+          <t>10/08/2022</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>00:24</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>23:01</t>
+          <t>23:15</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>00:49</t>
+          <t>01:00</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>03:32</t>
+          <t>03:45</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -1728,7 +1728,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>DEB_71270_10/08/2022</t>
+          <t>DEB_71270_11/08/2022</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1738,12 +1738,12 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>10/08/2022</t>
+          <t>11/08/2022</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>10:25</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>03:07</t>
+          <t>03:15</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>21:48</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1827,7 +1827,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>00:30</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12:24</t>
+          <t>12:30</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>12:09</t>
+          <t>12:15</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -1911,7 +1911,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>04:02</t>
+          <t>04:15</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -1939,7 +1939,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -1952,7 +1952,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>DEB_44250_12/08/2022</t>
+          <t>DEB_44250_11/08/2022</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1962,12 +1962,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>12/08/2022</t>
+          <t>11/08/2022</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>00:24</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>17:19</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12:54</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E57" t="n">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13:43</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="E58" t="n">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>18:43</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="E59" t="n">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>03:47</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="E61" t="n">
@@ -2163,7 +2163,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>20:33</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>23:01</t>
+          <t>23:15</t>
         </is>
       </c>
       <c r="E63" t="n">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>00:49</t>
+          <t>01:00</t>
         </is>
       </c>
       <c r="E64" t="n">
@@ -2247,7 +2247,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12:39</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="E65" t="n">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>22:28</t>
+          <t>22:30</t>
         </is>
       </c>
       <c r="E67" t="n">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>03:32</t>
+          <t>03:45</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>22:43</t>
+          <t>22:15</t>
         </is>
       </c>
       <c r="E69" t="n">
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>03:07</t>
+          <t>03:15</t>
         </is>
       </c>
       <c r="E70" t="n">
@@ -2415,7 +2415,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>21:48</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E71" t="n">
@@ -2443,7 +2443,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>23:33</t>
+          <t>23:45</t>
         </is>
       </c>
       <c r="E72" t="n">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>12:04</t>
+          <t>12:15</t>
         </is>
       </c>
       <c r="E73" t="n">
@@ -2499,7 +2499,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="E74" t="n">
@@ -2527,7 +2527,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E75" t="n">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>02:13</t>
+          <t>02:15</t>
         </is>
       </c>
       <c r="E76" t="n">
@@ -2568,7 +2568,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>DEB_44250_13/08/2022</t>
+          <t>DEB_44250_12/08/2022</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2578,12 +2578,12 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>09:59</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="E77" t="n">
@@ -2596,7 +2596,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>DEB_44865_13/08/2022</t>
+          <t>DEB_44865_12/08/2022</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2606,12 +2606,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>09:44</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="E78" t="n">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E79" t="n">
@@ -2667,7 +2667,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E80" t="n">
@@ -2695,7 +2695,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>13:43</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="E81" t="n">
@@ -2708,7 +2708,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>DEB_47214_13/08/2022</t>
+          <t>DEB_47214_12/08/2022</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2718,12 +2718,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>09:29</t>
+          <t>18:45</t>
         </is>
       </c>
       <c r="E82" t="n">
@@ -2751,7 +2751,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>10:02</t>
+          <t>10:15</t>
         </is>
       </c>
       <c r="E83" t="n">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>20:33</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="E84" t="n">
@@ -2807,7 +2807,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>08:43</t>
+          <t>08:45</t>
         </is>
       </c>
       <c r="E85" t="n">
@@ -2835,7 +2835,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="E86" t="n">
@@ -2863,7 +2863,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>22:36</t>
+          <t>22:45</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -2891,7 +2891,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>23:01</t>
+          <t>23:15</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -2919,7 +2919,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>00:24</t>
+          <t>00:15</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -2975,7 +2975,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>03:32</t>
+          <t>03:45</t>
         </is>
       </c>
       <c r="E91" t="n">
@@ -3031,7 +3031,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>02:36</t>
+          <t>02:30</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>03:07</t>
+          <t>03:15</t>
         </is>
       </c>
       <c r="E94" t="n">
@@ -3087,7 +3087,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>23:16</t>
+          <t>23:30</t>
         </is>
       </c>
       <c r="E95" t="n">
@@ -3115,7 +3115,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>06:03</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="E96" t="n">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>21:31</t>
+          <t>21:45</t>
         </is>
       </c>
       <c r="E97" t="n">
@@ -3156,7 +3156,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>DEB_44228_14/08/2022</t>
+          <t>DEB_44228_13/08/2022</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3166,12 +3166,12 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>14/08/2022</t>
+          <t>13/08/2022</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>00:09</t>
+          <t>02:15</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -3199,7 +3199,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>11:31</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="E99" t="n">
@@ -3227,7 +3227,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>21:16</t>
+          <t>21:30</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -3255,7 +3255,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>12:51</t>
+          <t>21:15</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -3283,7 +3283,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>02:51</t>
+          <t>03:00</t>
         </is>
       </c>
       <c r="E102" t="n">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>10:17</t>
+          <t>10:30</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -3339,7 +3339,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>22:00</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -3367,7 +3367,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>12:33</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -3395,7 +3395,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>23:01</t>
+          <t>23:15</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -3423,7 +3423,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>00:49</t>
+          <t>01:00</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -3507,7 +3507,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>03:32</t>
+          <t>03:45</t>
         </is>
       </c>
       <c r="E110" t="n">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>03:35</t>
+          <t>03:45</t>
         </is>
       </c>
       <c r="E112" t="n">
@@ -3591,7 +3591,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>04:17</t>
+          <t>04:30</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -3619,7 +3619,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>07:02</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="E114" t="n">
@@ -3703,7 +3703,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>00:50</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="E117" t="n">
@@ -3731,7 +3731,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>03:35</t>
+          <t>20:15</t>
         </is>
       </c>
       <c r="E118" t="n">
@@ -3759,7 +3759,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>01:05</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -3787,7 +3787,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>03:50</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -3815,7 +3815,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>01:35</t>
+          <t>01:15</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -3843,7 +3843,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>04:20</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E122" t="n">
@@ -3871,7 +3871,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>04:02</t>
+          <t>04:15</t>
         </is>
       </c>
       <c r="E123" t="n">
@@ -3899,7 +3899,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>06:47</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="E124" t="n">
@@ -3927,7 +3927,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>14:36</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="E125" t="n">
@@ -3955,7 +3955,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="E126" t="n">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>15:21</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E127" t="n">
@@ -4011,7 +4011,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>18:06</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="E128" t="n">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>14:51</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="E129" t="n">
@@ -4067,7 +4067,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="E130" t="n">
@@ -4095,7 +4095,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>22:43</t>
+          <t>22:45</t>
         </is>
       </c>
       <c r="E131" t="n">
@@ -4123,7 +4123,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>01:28</t>
+          <t>01:30</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -4151,7 +4151,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>01:20</t>
+          <t>01:00</t>
         </is>
       </c>
       <c r="E133" t="n">
@@ -4179,7 +4179,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>04:05</t>
+          <t>03:45</t>
         </is>
       </c>
       <c r="E134" t="n">
@@ -4207,7 +4207,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E135" t="n">
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>21:50</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="E136" t="n">
@@ -4263,7 +4263,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>02:51</t>
+          <t>02:45</t>
         </is>
       </c>
       <c r="E137" t="n">
@@ -4291,7 +4291,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>05:36</t>
+          <t>05:30</t>
         </is>
       </c>
       <c r="E138" t="n">
@@ -4319,7 +4319,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>04:32</t>
+          <t>03:45</t>
         </is>
       </c>
       <c r="E139" t="n">
@@ -4347,7 +4347,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>07:17</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="E140" t="n">
@@ -4375,7 +4375,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>22:58</t>
+          <t>23:00</t>
         </is>
       </c>
       <c r="E141" t="n">
@@ -4403,7 +4403,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>01:43</t>
+          <t>01:45</t>
         </is>
       </c>
       <c r="E142" t="n">
@@ -4431,7 +4431,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>15:06</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="E143" t="n">
@@ -4459,7 +4459,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="E144" t="n">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="E145" t="n">
@@ -4515,7 +4515,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="E146" t="n">
@@ -4584,7 +4584,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>FOR_450226_09/08/2022</t>
+          <t>FOR_450226_10/08/2022</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4594,12 +4594,12 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>09/08/2022</t>
+          <t>10/08/2022</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>23:46</t>
+          <t>03:45</t>
         </is>
       </c>
       <c r="E149" t="n">
@@ -4627,7 +4627,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>02:31</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="E150" t="n">
@@ -4655,7 +4655,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>16:27</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="E151" t="n">
@@ -4683,7 +4683,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="E152" t="n">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>03:47</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E153" t="n">
@@ -4739,7 +4739,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>06:32</t>
+          <t>06:45</t>
         </is>
       </c>
       <c r="E154" t="n">
@@ -4767,7 +4767,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>03:22</t>
+          <t>03:30</t>
         </is>
       </c>
       <c r="E155" t="n">
@@ -4795,7 +4795,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>06:07</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="E156" t="n">
@@ -4823,7 +4823,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>04:17</t>
+          <t>04:30</t>
         </is>
       </c>
       <c r="E157" t="n">
@@ -4851,7 +4851,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>07:02</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="E158" t="n">
@@ -4879,7 +4879,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>01:04</t>
+          <t>01:15</t>
         </is>
       </c>
       <c r="E159" t="n">
@@ -4907,7 +4907,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>03:49</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E160" t="n">
@@ -4935,7 +4935,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>14:35</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="E161" t="n">
@@ -4963,7 +4963,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>02:45</t>
         </is>
       </c>
       <c r="E162" t="n">
@@ -4991,7 +4991,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>23:31</t>
+          <t>23:30</t>
         </is>
       </c>
       <c r="E163" t="n">
@@ -5019,7 +5019,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>02:16</t>
+          <t>02:15</t>
         </is>
       </c>
       <c r="E164" t="n">
@@ -5047,7 +5047,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>13:58</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E165" t="n">
@@ -5075,7 +5075,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="E166" t="n">
@@ -5159,7 +5159,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="E169" t="n">
@@ -5187,7 +5187,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>15:32</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="E170" t="n">
@@ -5215,7 +5215,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="E171" t="n">
@@ -5243,7 +5243,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>15:47</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E172" t="n">
@@ -5271,7 +5271,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>03:22</t>
+          <t>03:30</t>
         </is>
       </c>
       <c r="E173" t="n">
@@ -5299,7 +5299,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>06:07</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="E174" t="n">
@@ -5327,7 +5327,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>00:39</t>
+          <t>00:30</t>
         </is>
       </c>
       <c r="E175" t="n">
@@ -5355,7 +5355,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>03:24</t>
+          <t>03:15</t>
         </is>
       </c>
       <c r="E176" t="n">
@@ -5368,7 +5368,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>FOR_54053_09/08/2022</t>
+          <t>FOR_54053_10/08/2022</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -5378,12 +5378,12 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>09/08/2022</t>
+          <t>10/08/2022</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>23:16</t>
+          <t>12:15</t>
         </is>
       </c>
       <c r="E177" t="n">
@@ -5411,7 +5411,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>02:01</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E178" t="n">
@@ -5439,7 +5439,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>04:02</t>
+          <t>04:15</t>
         </is>
       </c>
       <c r="E179" t="n">
@@ -5467,7 +5467,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>06:47</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="E180" t="n">
@@ -5495,7 +5495,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>00:01</t>
+          <t>00:15</t>
         </is>
       </c>
       <c r="E181" t="n">
@@ -5523,7 +5523,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>02:46</t>
+          <t>03:00</t>
         </is>
       </c>
       <c r="E182" t="n">
@@ -5551,7 +5551,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>23:31</t>
+          <t>23:45</t>
         </is>
       </c>
       <c r="E183" t="n">
@@ -5579,7 +5579,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>02:16</t>
+          <t>02:30</t>
         </is>
       </c>
       <c r="E184" t="n">
@@ -5607,7 +5607,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>23:16</t>
+          <t>23:30</t>
         </is>
       </c>
       <c r="E185" t="n">
@@ -5635,7 +5635,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>23:11</t>
+          <t>02:15</t>
         </is>
       </c>
       <c r="E186" t="n">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>04:02</t>
+          <t>04:15</t>
         </is>
       </c>
       <c r="E187" t="n">
@@ -5691,7 +5691,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>06:47</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="E188" t="n">
@@ -5719,7 +5719,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>04:17</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="E189" t="n">
@@ -5747,7 +5747,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>07:02</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="E190" t="n">
@@ -5760,7 +5760,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>FOR_44203_10/08/2022</t>
+          <t>FOR_44203_11/08/2022</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -5770,12 +5770,12 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>10/08/2022</t>
+          <t>11/08/2022</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>22:30</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="E191" t="n">
@@ -5803,7 +5803,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>01:15</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="E192" t="n">
@@ -5887,7 +5887,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>01:58</t>
+          <t>01:45</t>
         </is>
       </c>
       <c r="E195" t="n">
@@ -5915,7 +5915,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>04:43</t>
+          <t>04:30</t>
         </is>
       </c>
       <c r="E196" t="n">
@@ -5943,7 +5943,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>03:47</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E197" t="n">
@@ -5971,7 +5971,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>06:32</t>
+          <t>06:45</t>
         </is>
       </c>
       <c r="E198" t="n">
@@ -5999,7 +5999,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>11:23</t>
+          <t>11:15</t>
         </is>
       </c>
       <c r="E199" t="n">
@@ -6027,7 +6027,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>14:08</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E200" t="n">
@@ -6040,7 +6040,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>FOR_47247_11/08/2022</t>
+          <t>FOR_47247_10/08/2022</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -6050,12 +6050,12 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>11/08/2022</t>
+          <t>10/08/2022</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>07:40</t>
+          <t>22:30</t>
         </is>
       </c>
       <c r="E201" t="n">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>10:25</t>
+          <t>01:15</t>
         </is>
       </c>
       <c r="E202" t="n">
@@ -6111,7 +6111,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>01:19</t>
+          <t>01:30</t>
         </is>
       </c>
       <c r="E203" t="n">
@@ -6139,7 +6139,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>04:04</t>
+          <t>04:15</t>
         </is>
       </c>
       <c r="E204" t="n">
@@ -6223,7 +6223,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>03:22</t>
+          <t>03:30</t>
         </is>
       </c>
       <c r="E207" t="n">
@@ -6251,7 +6251,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>06:07</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="E208" t="n">
@@ -6264,7 +6264,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>FOR_54003_11/08/2022</t>
+          <t>FOR_54003_10/08/2022</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -6274,12 +6274,12 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>11/08/2022</t>
+          <t>10/08/2022</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>00:39</t>
+          <t>22:15</t>
         </is>
       </c>
       <c r="E209" t="n">
@@ -6307,7 +6307,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>03:24</t>
+          <t>01:00</t>
         </is>
       </c>
       <c r="E210" t="n">
@@ -6320,7 +6320,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>FOR_54051_10/08/2022</t>
+          <t>FOR_54051_11/08/2022</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -6330,12 +6330,12 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>10/08/2022</t>
+          <t>11/08/2022</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>23:48</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="E211" t="n">
@@ -6363,7 +6363,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>02:33</t>
+          <t>02:45</t>
         </is>
       </c>
       <c r="E212" t="n">
@@ -6391,7 +6391,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>13:02</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="E213" t="n">
@@ -6419,7 +6419,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>15:47</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E214" t="n">
@@ -6503,7 +6503,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>23:01</t>
+          <t>23:00</t>
         </is>
       </c>
       <c r="E217" t="n">
@@ -6531,7 +6531,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>01:46</t>
+          <t>01:45</t>
         </is>
       </c>
       <c r="E218" t="n">
@@ -6559,7 +6559,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E219" t="n">
@@ -6587,7 +6587,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>15:33</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="E220" t="n">
@@ -6615,7 +6615,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>19:26</t>
+          <t>13:45</t>
         </is>
       </c>
       <c r="E221" t="n">
@@ -6643,7 +6643,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>22:11</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="E222" t="n">
@@ -6671,7 +6671,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>03:47</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E223" t="n">
@@ -6699,7 +6699,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>06:32</t>
+          <t>06:45</t>
         </is>
       </c>
       <c r="E224" t="n">
@@ -6727,7 +6727,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>01:04</t>
+          <t>01:15</t>
         </is>
       </c>
       <c r="E225" t="n">
@@ -6755,7 +6755,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>03:49</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E226" t="n">
@@ -6783,7 +6783,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>22:58</t>
+          <t>22:30</t>
         </is>
       </c>
       <c r="E227" t="n">
@@ -6811,7 +6811,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>01:43</t>
+          <t>01:15</t>
         </is>
       </c>
       <c r="E228" t="n">
@@ -6839,7 +6839,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>23:16</t>
+          <t>23:30</t>
         </is>
       </c>
       <c r="E229" t="n">
@@ -6867,7 +6867,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>12:47</t>
+          <t>02:15</t>
         </is>
       </c>
       <c r="E230" t="n">
@@ -6895,7 +6895,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>23:47</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E231" t="n">
@@ -6908,7 +6908,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>DEG_44249_12/08/2022</t>
+          <t>DEG_44249_11/08/2022</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -6918,12 +6918,12 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>12/08/2022</t>
+          <t>11/08/2022</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>02:32</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="E232" t="n">
@@ -6951,7 +6951,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>03:47</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E233" t="n">
@@ -6979,7 +6979,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>06:32</t>
+          <t>06:45</t>
         </is>
       </c>
       <c r="E234" t="n">
@@ -7063,7 +7063,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>13:24</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="E237" t="n">
@@ -7091,7 +7091,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>16:09</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="E238" t="n">
@@ -7119,7 +7119,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>01:04</t>
+          <t>01:15</t>
         </is>
       </c>
       <c r="E239" t="n">
@@ -7147,7 +7147,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>03:49</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E240" t="n">
@@ -7175,7 +7175,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>09:13</t>
+          <t>09:15</t>
         </is>
       </c>
       <c r="E241" t="n">
@@ -7203,7 +7203,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E242" t="n">
@@ -7216,7 +7216,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>FOR_54003_12/08/2022</t>
+          <t>FOR_54003_11/08/2022</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -7226,12 +7226,12 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>12/08/2022</t>
+          <t>11/08/2022</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>00:39</t>
+          <t>23:00</t>
         </is>
       </c>
       <c r="E243" t="n">
@@ -7259,7 +7259,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>03:24</t>
+          <t>01:45</t>
         </is>
       </c>
       <c r="E244" t="n">
@@ -7287,7 +7287,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>02:28</t>
+          <t>02:30</t>
         </is>
       </c>
       <c r="E245" t="n">
@@ -7315,7 +7315,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>05:13</t>
+          <t>05:15</t>
         </is>
       </c>
       <c r="E246" t="n">
@@ -7343,7 +7343,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>13:09</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="E247" t="n">
@@ -7371,7 +7371,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>15:54</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E248" t="n">
@@ -7399,7 +7399,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>06:18</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="E249" t="n">
@@ -7427,7 +7427,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>09:03</t>
+          <t>09:15</t>
         </is>
       </c>
       <c r="E250" t="n">
@@ -7455,7 +7455,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="E251" t="n">
@@ -7483,7 +7483,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="E252" t="n">
@@ -7511,7 +7511,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>23:23</t>
+          <t>13:15</t>
         </is>
       </c>
       <c r="E253" t="n">
@@ -7524,7 +7524,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>DEG_41258_13/08/2022</t>
+          <t>DEG_41258_12/08/2022</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -7534,12 +7534,12 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>02:08</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="E254" t="n">
@@ -7567,7 +7567,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>03:22</t>
+          <t>03:30</t>
         </is>
       </c>
       <c r="E255" t="n">
@@ -7595,7 +7595,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>06:07</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="E256" t="n">
@@ -7679,7 +7679,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>22:51</t>
+          <t>23:00</t>
         </is>
       </c>
       <c r="E259" t="n">
@@ -7707,7 +7707,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>03:55</t>
+          <t>01:45</t>
         </is>
       </c>
       <c r="E260" t="n">
@@ -7735,7 +7735,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>04:17</t>
+          <t>04:30</t>
         </is>
       </c>
       <c r="E261" t="n">
@@ -7763,7 +7763,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>07:02</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="E262" t="n">
@@ -7791,7 +7791,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>00:03</t>
+          <t>00:15</t>
         </is>
       </c>
       <c r="E263" t="n">
@@ -7819,7 +7819,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>02:48</t>
+          <t>03:00</t>
         </is>
       </c>
       <c r="E264" t="n">
@@ -7832,7 +7832,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>FOR_47281_12/08/2022</t>
+          <t>FOR_47281_13/08/2022</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -7842,12 +7842,12 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>12/08/2022</t>
+          <t>13/08/2022</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>23:48</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="E265" t="n">
@@ -7875,7 +7875,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>02:33</t>
+          <t>02:45</t>
         </is>
       </c>
       <c r="E266" t="n">
@@ -7903,7 +7903,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>21:48</t>
+          <t>20:15</t>
         </is>
       </c>
       <c r="E267" t="n">
@@ -7916,7 +7916,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>DEG_489044_13/08/2022</t>
+          <t>DEG_489044_12/08/2022</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -7926,12 +7926,12 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>00:33</t>
+          <t>23:00</t>
         </is>
       </c>
       <c r="E268" t="n">
@@ -7944,7 +7944,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>FOR_489119_13/08/2022</t>
+          <t>FOR_489119_12/08/2022</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -7954,12 +7954,12 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>10:14</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E269" t="n">
@@ -7972,7 +7972,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>DEG_489119_13/08/2022</t>
+          <t>DEG_489119_12/08/2022</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -7982,12 +7982,12 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>12:59</t>
+          <t>23:45</t>
         </is>
       </c>
       <c r="E270" t="n">
@@ -8015,7 +8015,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>02:51</t>
+          <t>02:45</t>
         </is>
       </c>
       <c r="E271" t="n">
@@ -8043,7 +8043,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>05:36</t>
+          <t>05:30</t>
         </is>
       </c>
       <c r="E272" t="n">
@@ -8071,7 +8071,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>08:58</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="E273" t="n">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>11:43</t>
+          <t>11:45</t>
         </is>
       </c>
       <c r="E274" t="n">
@@ -8112,7 +8112,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>FOR_54086_13/08/2022</t>
+          <t>FOR_54086_12/08/2022</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -8122,12 +8122,12 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>00:30</t>
+          <t>00:45</t>
         </is>
       </c>
       <c r="E275" t="n">
@@ -8140,7 +8140,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>DEG_54086_13/08/2022</t>
+          <t>DEG_54086_12/08/2022</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -8150,12 +8150,12 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>03:15</t>
+          <t>03:30</t>
         </is>
       </c>
       <c r="E276" t="n">
@@ -8183,7 +8183,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>23:31</t>
+          <t>23:30</t>
         </is>
       </c>
       <c r="E277" t="n">
@@ -8211,7 +8211,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>02:16</t>
+          <t>02:15</t>
         </is>
       </c>
       <c r="E278" t="n">
@@ -8239,7 +8239,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>01:19</t>
+          <t>01:15</t>
         </is>
       </c>
       <c r="E279" t="n">
@@ -8267,7 +8267,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>04:04</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E280" t="n">
@@ -8351,7 +8351,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>01:04</t>
+          <t>01:30</t>
         </is>
       </c>
       <c r="E283" t="n">
@@ -8379,7 +8379,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>03:49</t>
+          <t>04:15</t>
         </is>
       </c>
       <c r="E284" t="n">
@@ -8392,7 +8392,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>FOR_489447_14/08/2022</t>
+          <t>FOR_489447_12/08/2022</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -8402,12 +8402,12 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>14/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>02:51</t>
+          <t>23:30</t>
         </is>
       </c>
       <c r="E285" t="n">
@@ -8420,7 +8420,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>DEG_489447_14/08/2022</t>
+          <t>DEG_489447_13/08/2022</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -8430,12 +8430,12 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>14/08/2022</t>
+          <t>13/08/2022</t>
         </is>
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>05:36</t>
+          <t>02:15</t>
         </is>
       </c>
       <c r="E286" t="n">
@@ -8463,7 +8463,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>00:39</t>
+          <t>00:30</t>
         </is>
       </c>
       <c r="E287" t="n">
@@ -8491,7 +8491,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>03:24</t>
+          <t>03:15</t>
         </is>
       </c>
       <c r="E288" t="n">
@@ -8519,7 +8519,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>23:46</t>
+          <t>23:45</t>
         </is>
       </c>
       <c r="E289" t="n">
@@ -8547,7 +8547,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>02:31</t>
+          <t>02:30</t>
         </is>
       </c>
       <c r="E290" t="n">
@@ -8575,7 +8575,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>03:06</t>
+          <t>03:15</t>
         </is>
       </c>
       <c r="E291" t="n">
@@ -8603,7 +8603,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>05:51</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="E292" t="n">
@@ -8631,7 +8631,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>03:22</t>
+          <t>03:30</t>
         </is>
       </c>
       <c r="E293" t="n">
@@ -8659,7 +8659,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>06:07</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="E294" t="n">
@@ -8687,7 +8687,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>04:20</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E295" t="n">
@@ -8715,7 +8715,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>07:05</t>
+          <t>06:45</t>
         </is>
       </c>
       <c r="E296" t="n">
@@ -8743,7 +8743,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>00:54</t>
+          <t>04:45</t>
         </is>
       </c>
       <c r="E297" t="n">
@@ -8771,7 +8771,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>03:39</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="E298" t="n">
@@ -8799,7 +8799,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>04:02</t>
+          <t>04:00</t>
         </is>
       </c>
       <c r="E299" t="n">
@@ -8812,7 +8812,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>DEG_431121_15/08/2022</t>
+          <t>DEG_431121_13/08/2022</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -8822,12 +8822,12 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>15/08/2022</t>
+          <t>13/08/2022</t>
         </is>
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>02:54</t>
+          <t>06:45</t>
         </is>
       </c>
       <c r="E300" t="n">
@@ -8840,7 +8840,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>FOR_450226_14/08/2022</t>
+          <t>FOR_450226_15/08/2022</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -8850,12 +8850,12 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>14/08/2022</t>
+          <t>15/08/2022</t>
         </is>
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>23:54</t>
+          <t>01:45</t>
         </is>
       </c>
       <c r="E301" t="n">
@@ -8883,7 +8883,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>02:39</t>
+          <t>04:30</t>
         </is>
       </c>
       <c r="E302" t="n">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>03:47</t>
+          <t>04:15</t>
         </is>
       </c>
       <c r="E303" t="n">
@@ -8924,7 +8924,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>DEG_489447_13/08/2022</t>
+          <t>DEG_489447_15/08/2022</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -8934,12 +8934,12 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>15/08/2022</t>
         </is>
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>06:32</t>
+          <t>04:45</t>
         </is>
       </c>
       <c r="E304" t="n">
@@ -8967,7 +8967,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>04:05</t>
+          <t>04:30</t>
         </is>
       </c>
       <c r="E305" t="n">
@@ -8995,7 +8995,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>06:50</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="E306" t="n">
@@ -9008,7 +9008,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>FOR_54051_15/08/2022</t>
+          <t>FOR_54051_13/08/2022</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -9018,12 +9018,12 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>15/08/2022</t>
+          <t>13/08/2022</t>
         </is>
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>00:24</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="E307" t="n">
@@ -9036,7 +9036,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>DEG_54051_15/08/2022</t>
+          <t>DEG_54051_13/08/2022</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -9046,12 +9046,12 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>15/08/2022</t>
+          <t>13/08/2022</t>
         </is>
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>03:09</t>
+          <t>09:15</t>
         </is>
       </c>
       <c r="E308" t="n">
@@ -9079,7 +9079,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>03:50</t>
+          <t>04:15</t>
         </is>
       </c>
       <c r="E309" t="n">
@@ -9107,7 +9107,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>06:35</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="E310" t="n">
@@ -9120,7 +9120,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>FOR_54231_13/08/2022</t>
+          <t>FOR_54231_15/08/2022</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -9130,12 +9130,12 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>15/08/2022</t>
         </is>
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>23:16</t>
+          <t>04:30</t>
         </is>
       </c>
       <c r="E311" t="n">
@@ -9148,7 +9148,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>DEG_54231_14/08/2022</t>
+          <t>DEG_54231_15/08/2022</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
@@ -9158,12 +9158,12 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>14/08/2022</t>
+          <t>15/08/2022</t>
         </is>
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>02:01</t>
+          <t>13:30</t>
         </is>
       </c>
       <c r="E312" t="n">
@@ -9176,7 +9176,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>FOR_41258_14/08/2022</t>
+          <t>FOR_41258_15/08/2022</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -9186,12 +9186,12 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>14/08/2022</t>
+          <t>15/08/2022</t>
         </is>
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>23:39</t>
+          <t>23:15</t>
         </is>
       </c>
       <c r="E313" t="n">
@@ -9204,7 +9204,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>DEG_41258_15/08/2022</t>
+          <t>DEG_41258_16/08/2022</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
@@ -9214,12 +9214,12 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>15/08/2022</t>
+          <t>16/08/2022</t>
         </is>
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>02:24</t>
+          <t>02:00</t>
         </is>
       </c>
       <c r="E314" t="n">
@@ -9232,7 +9232,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>FOR_431091_15/08/2022</t>
+          <t>FOR_431091_12/08/2022</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -9242,12 +9242,12 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>15/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>00:39</t>
+          <t>12:30</t>
         </is>
       </c>
       <c r="E315" t="n">
@@ -9260,7 +9260,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>DEG_431091_15/08/2022</t>
+          <t>DEG_431091_12/08/2022</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -9270,12 +9270,12 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>15/08/2022</t>
+          <t>12/08/2022</t>
         </is>
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>03:24</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="E316" t="n">
@@ -9303,7 +9303,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>21:15</t>
         </is>
       </c>
       <c r="E317" t="n">
@@ -9316,7 +9316,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>DEG_489044_13/08/2022</t>
+          <t>DEG_489044_14/08/2022</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -9326,12 +9326,12 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>13/08/2022</t>
+          <t>14/08/2022</t>
         </is>
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>21:01</t>
+          <t>00:00</t>
         </is>
       </c>
       <c r="E318" t="n">
@@ -9359,7 +9359,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>22:43</t>
+          <t>22:45</t>
         </is>
       </c>
       <c r="E319" t="n">
@@ -9387,7 +9387,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>01:28</t>
+          <t>01:30</t>
         </is>
       </c>
       <c r="E320" t="n">

</xml_diff>